<commit_message>
Integrated Demand Model to ModelCenter
</commit_message>
<xml_diff>
--- a/Boils_per_Charge/Boils_per_Charge.xlsx
+++ b/Boils_per_Charge/Boils_per_Charge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07531a99d7244c5b/Documents/GitHub/ASE6002PEK/Boils_per_Charge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{E1B203CD-980D-4B68-9256-E22E05DA1089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1550A2A-B7C6-44FC-B31B-ED2AAA8B5B84}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{E1B203CD-980D-4B68-9256-E22E05DA1089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C938CE-5F89-45A7-8880-20B2A1A2326F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5040" windowWidth="38700" windowHeight="15345" xr2:uid="{8DE6D8F7-A165-49AB-ACB4-90769F3729E6}"/>
+    <workbookView xWindow="2055" yWindow="5430" windowWidth="38700" windowHeight="15345" xr2:uid="{8DE6D8F7-A165-49AB-ACB4-90769F3729E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,6 +109,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,7 +453,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>599400000</v>
+        <v>599400</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -465,7 +469,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>142.39780273333301</v>
+        <v>320.39505615000002</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -474,7 +478,7 @@
       </c>
       <c r="B6">
         <f>B3/(B4*B5)</f>
-        <v>2806.2230759861309</v>
+        <v>1.247210255993833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>